<commit_message>
Se realizan cambios para sanity semilla 9
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -222,12 +222,6 @@
     <t>732111324707275</t>
   </si>
   <si>
-    <t>3045984642</t>
-  </si>
-  <si>
-    <t>732111193278730</t>
-  </si>
-  <si>
     <t>81670</t>
   </si>
   <si>
@@ -298,6 +292,12 @@
   </si>
   <si>
     <t>99299424</t>
+  </si>
+  <si>
+    <t>3045981670</t>
+  </si>
+  <si>
+    <t>732111193278811</t>
   </si>
 </sst>
 </file>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -947,6 +947,7 @@
     <col min="3" max="3" width="30.1796875" customWidth="1"/>
     <col min="4" max="4" width="28.1796875" customWidth="1"/>
     <col min="5" max="5" width="35.81640625" customWidth="1"/>
+    <col min="6" max="6" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
@@ -980,13 +981,13 @@
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -1020,10 +1021,10 @@
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
@@ -1043,7 +1044,7 @@
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>46</v>
@@ -1055,7 +1056,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>50</v>
@@ -1066,7 +1067,7 @@
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>19</v>
@@ -1083,10 +1084,10 @@
         <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>23</v>
@@ -1126,7 +1127,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>56</v>
@@ -1135,7 +1136,7 @@
         <v>57</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>59</v>
@@ -1155,7 +1156,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>63</v>
@@ -1164,19 +1165,19 @@
         <v>64</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1">
@@ -1184,7 +1185,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>56</v>
@@ -1198,13 +1199,13 @@
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1">
@@ -1212,13 +1213,13 @@
         <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1226,13 +1227,13 @@
         <v>31</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>